<commit_message>
Updating Test Data sheet
</commit_message>
<xml_diff>
--- a/Facebook/Test Data/TestData.xlsx
+++ b/Facebook/Test Data/TestData.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Enter your user name</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter your password</t>
+    <t xml:space="preserve">Enter your password here</t>
   </si>
 </sst>
 </file>
@@ -142,14 +142,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>

</xml_diff>